<commit_message>
Normalize the input files, capacity column
</commit_message>
<xml_diff>
--- a/RoomList.xlsx
+++ b/RoomList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THAC SI\Algorithm and PS\Timetabling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoangloctran/Documents/Algorithm and PS/Timetabling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE97441-78BE-4FD7-8862-30650F20DEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520A424A-3B1C-C742-83F7-7A4CE6779ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23010" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{B1EEB453-3345-4BD9-9501-33C83FEF5E6D}"/>
+    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" activeTab="1" xr2:uid="{B1EEB453-3345-4BD9-9501-33C83FEF5E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="123">
   <si>
     <t>RoomName</t>
   </si>
@@ -99,9 +99,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>CQDT</t>
-  </si>
-  <si>
     <t>B1.02</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>E11.8</t>
+  </si>
+  <si>
+    <t>CQUI</t>
   </si>
 </sst>
 </file>
@@ -756,16 +756,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B7C885-A034-431A-8F8D-4E04EFE689AF}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -787,7 +787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -798,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -809,7 +809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -820,7 +820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -831,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -842,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -853,7 +853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -864,7 +864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -875,7 +875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -886,7 +886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -897,7 +897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -908,7 +908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -916,10 +916,10 @@
         <v>400</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -927,10 +927,10 @@
         <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -938,155 +938,155 @@
         <v>200</v>
       </c>
       <c r="C16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
       </c>
       <c r="B17">
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B26">
-        <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
-        <v>72</v>
-      </c>
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
-        <v>50</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>34</v>
-      </c>
-      <c r="B29">
-        <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
       </c>
       <c r="B30">
         <v>64</v>
@@ -1095,31 +1095,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
-        <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>37</v>
-      </c>
-      <c r="B32">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>38</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -1128,9 +1128,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>32</v>
@@ -1139,9 +1139,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
         <v>32</v>
@@ -1150,9 +1150,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>32</v>
@@ -1161,86 +1161,86 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B40">
-        <v>72</v>
-      </c>
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41">
+        <v>72</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B41">
-        <v>72</v>
-      </c>
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="B42">
-        <v>72</v>
-      </c>
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>48</v>
-      </c>
-      <c r="B43">
-        <v>72</v>
-      </c>
-      <c r="C43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>49</v>
       </c>
       <c r="B44">
         <v>32</v>
@@ -1249,9 +1249,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <v>32</v>
@@ -1260,9 +1260,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46">
         <v>32</v>
@@ -1271,9 +1271,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47">
         <v>32</v>
@@ -1282,75 +1282,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>160</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>56</v>
       </c>
-      <c r="B51">
-        <v>72</v>
-      </c>
-      <c r="C51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52">
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>57</v>
       </c>
-      <c r="B52">
-        <v>72</v>
-      </c>
-      <c r="C52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B53">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>58</v>
-      </c>
-      <c r="B53">
-        <v>72</v>
-      </c>
-      <c r="C53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>59</v>
       </c>
       <c r="B54">
         <v>64</v>
@@ -1359,163 +1359,163 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56">
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>61</v>
       </c>
-      <c r="B56">
-        <v>72</v>
-      </c>
-      <c r="C56" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>62</v>
-      </c>
-      <c r="B57">
-        <v>72</v>
-      </c>
-      <c r="C57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>63</v>
       </c>
       <c r="B58">
         <v>180</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59">
         <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60">
         <v>64</v>
       </c>
       <c r="C60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61">
         <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>67</v>
       </c>
-      <c r="B62">
-        <v>72</v>
-      </c>
-      <c r="C62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>68</v>
-      </c>
-      <c r="B63">
-        <v>72</v>
-      </c>
-      <c r="C63" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>69</v>
       </c>
       <c r="B64">
         <v>192</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65">
+        <v>72</v>
+      </c>
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>70</v>
       </c>
-      <c r="B65">
-        <v>72</v>
-      </c>
-      <c r="C65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66">
+        <v>72</v>
+      </c>
+      <c r="C66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>71</v>
-      </c>
-      <c r="B66">
-        <v>72</v>
-      </c>
-      <c r="C66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>72</v>
       </c>
       <c r="B67">
         <v>200</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68">
+        <v>50</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>73</v>
-      </c>
-      <c r="B68">
-        <v>50</v>
-      </c>
-      <c r="C68" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>74</v>
       </c>
       <c r="B69">
         <v>32</v>
@@ -1524,9 +1524,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70">
         <v>36</v>
@@ -1535,9 +1535,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71">
         <v>56</v>
@@ -1546,9 +1546,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72">
         <v>100</v>
@@ -1557,9 +1557,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73">
         <v>64</v>
@@ -1568,9 +1568,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>100</v>
@@ -1579,9 +1579,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75">
         <v>30</v>
@@ -1590,20 +1590,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>50</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>81</v>
-      </c>
-      <c r="B76">
-        <v>50</v>
-      </c>
-      <c r="C76" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>82</v>
       </c>
       <c r="B77">
         <v>100</v>
@@ -1612,42 +1612,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78">
         <v>140</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79">
         <v>140</v>
       </c>
       <c r="C79" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80">
+        <v>50</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>85</v>
-      </c>
-      <c r="B80">
-        <v>50</v>
-      </c>
-      <c r="C80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>86</v>
       </c>
       <c r="B81">
         <v>30</v>
@@ -1656,20 +1656,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B82">
         <v>100</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83">
         <v>56</v>
@@ -1678,9 +1678,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B84">
         <v>56</v>
@@ -1689,9 +1689,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85">
         <v>30</v>
@@ -1700,9 +1700,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B86">
         <v>56</v>
@@ -1711,20 +1711,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87">
+        <v>50</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>92</v>
-      </c>
-      <c r="B87">
-        <v>50</v>
-      </c>
-      <c r="C87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>93</v>
       </c>
       <c r="B88">
         <v>56</v>
@@ -1733,75 +1733,75 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>50</v>
+      </c>
+      <c r="C89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>94</v>
       </c>
-      <c r="B89">
-        <v>50</v>
-      </c>
-      <c r="C89" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B90">
+        <v>50</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>95</v>
       </c>
-      <c r="B90">
-        <v>50</v>
-      </c>
-      <c r="C90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B91">
+        <v>50</v>
+      </c>
+      <c r="C91" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>96</v>
       </c>
-      <c r="B91">
-        <v>50</v>
-      </c>
-      <c r="C91" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="B92">
+        <v>50</v>
+      </c>
+      <c r="C92" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>97</v>
       </c>
-      <c r="B92">
-        <v>50</v>
-      </c>
-      <c r="C92" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B93">
+        <v>50</v>
+      </c>
+      <c r="C93" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>98</v>
       </c>
-      <c r="B93">
-        <v>50</v>
-      </c>
-      <c r="C93" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B94">
+        <v>50</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>99</v>
-      </c>
-      <c r="B94">
-        <v>50</v>
-      </c>
-      <c r="C94" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>100</v>
       </c>
       <c r="B95">
         <v>30</v>
@@ -1810,64 +1810,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96">
         <v>140</v>
       </c>
       <c r="C96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97">
         <v>140</v>
       </c>
       <c r="C97" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98">
+        <v>50</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>103</v>
-      </c>
-      <c r="B98">
-        <v>50</v>
-      </c>
-      <c r="C98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>104</v>
       </c>
       <c r="B99">
         <v>140</v>
       </c>
       <c r="C99" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100">
+        <v>50</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>105</v>
-      </c>
-      <c r="B100">
-        <v>50</v>
-      </c>
-      <c r="C100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>106</v>
       </c>
       <c r="B101">
         <v>48</v>
@@ -1876,31 +1876,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102">
         <v>140</v>
       </c>
       <c r="C102" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B103">
         <v>140</v>
       </c>
       <c r="C103" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B104">
         <v>30</v>
@@ -1909,9 +1909,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B105">
         <v>48</v>
@@ -1920,9 +1920,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B106">
         <v>48</v>
@@ -1931,9 +1931,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B107">
         <v>30</v>
@@ -1942,9 +1942,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B108">
         <v>48</v>
@@ -1953,9 +1953,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B109">
         <v>54</v>
@@ -1964,9 +1964,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B110">
         <v>48</v>
@@ -1975,9 +1975,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B111">
         <v>30</v>
@@ -1986,9 +1986,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B112">
         <v>48</v>
@@ -1997,20 +1997,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B113">
+        <v>50</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>118</v>
-      </c>
-      <c r="B113">
-        <v>50</v>
-      </c>
-      <c r="C113" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>119</v>
       </c>
       <c r="B114">
         <v>32</v>
@@ -2019,9 +2019,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B115">
         <v>32</v>
@@ -2030,9 +2030,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B116">
         <v>32</v>
@@ -2041,9 +2041,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B117">
         <v>30</v>
@@ -2055,4 +2055,1313 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E35384-50AF-3948-8925-2CA814DA449B}">
+  <dimension ref="A1:C117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41">
+        <v>50</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47">
+        <v>52</v>
+      </c>
+      <c r="C47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>64</v>
+      </c>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>64</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>64</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56">
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61">
+        <v>72</v>
+      </c>
+      <c r="C61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64">
+        <v>72</v>
+      </c>
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65">
+        <v>72</v>
+      </c>
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66">
+        <v>72</v>
+      </c>
+      <c r="C66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>72</v>
+      </c>
+      <c r="C67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>72</v>
+      </c>
+      <c r="C68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>72</v>
+      </c>
+      <c r="C70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71">
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72">
+        <v>136</v>
+      </c>
+      <c r="C72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73">
+        <v>140</v>
+      </c>
+      <c r="C73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74">
+        <v>140</v>
+      </c>
+      <c r="C74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75">
+        <v>140</v>
+      </c>
+      <c r="C75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76">
+        <v>140</v>
+      </c>
+      <c r="C76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77">
+        <v>140</v>
+      </c>
+      <c r="C77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78">
+        <v>140</v>
+      </c>
+      <c r="C78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79">
+        <v>140</v>
+      </c>
+      <c r="C79" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80">
+        <v>140</v>
+      </c>
+      <c r="C80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81">
+        <v>140</v>
+      </c>
+      <c r="C81" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82">
+        <v>154</v>
+      </c>
+      <c r="C82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>54</v>
+      </c>
+      <c r="B83">
+        <v>160</v>
+      </c>
+      <c r="C83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>62</v>
+      </c>
+      <c r="B84">
+        <v>180</v>
+      </c>
+      <c r="C84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85">
+        <v>192</v>
+      </c>
+      <c r="C85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86">
+        <v>200</v>
+      </c>
+      <c r="C86" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87">
+        <v>200</v>
+      </c>
+      <c r="C87" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>71</v>
+      </c>
+      <c r="B88">
+        <v>200</v>
+      </c>
+      <c r="C88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89">
+        <v>400</v>
+      </c>
+      <c r="C89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90">
+        <v>30</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91">
+        <v>30</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92">
+        <v>30</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>99</v>
+      </c>
+      <c r="B93">
+        <v>30</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94">
+        <v>32</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>38</v>
+      </c>
+      <c r="B95">
+        <v>32</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>39</v>
+      </c>
+      <c r="B96">
+        <v>32</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>48</v>
+      </c>
+      <c r="B98">
+        <v>32</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>49</v>
+      </c>
+      <c r="B99">
+        <v>32</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>50</v>
+      </c>
+      <c r="B100">
+        <v>32</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101">
+        <v>32</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102">
+        <v>48</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>50</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>50</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105">
+        <v>50</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106">
+        <v>50</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B107">
+        <v>50</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>102</v>
+      </c>
+      <c r="B108">
+        <v>50</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109">
+        <v>50</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110">
+        <v>64</v>
+      </c>
+      <c r="C110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111">
+        <v>25</v>
+      </c>
+      <c r="C111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112">
+        <v>25</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113">
+        <v>30</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114">
+        <v>30</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>11</v>
+      </c>
+      <c r="B115">
+        <v>30</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116">
+        <v>30</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117">
+        <v>30</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C117">
+    <sortCondition ref="C2:C117"/>
+    <sortCondition ref="B2:B117"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>